<commit_message>
added version 2 for LRFR Template, focused on capacity
</commit_message>
<xml_diff>
--- a/docs/templates/LRFR_Template_v1.xlsx
+++ b/docs/templates/LRFR_Template_v1.xlsx
@@ -37,7 +37,7 @@
     <author>Nick</author>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0">
+    <comment ref="C4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -79,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B10" authorId="0">
+    <comment ref="A10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="A14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="A16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -1130,42 +1130,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1187,6 +1151,42 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1494,7 +1494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1505,12 +1505,12 @@
   <dimension ref="A1:N59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="29.42578125" style="11" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" style="13" customWidth="1"/>
     <col min="4" max="4" width="31.28515625" customWidth="1"/>
@@ -1535,308 +1535,282 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="18" t="s">
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="20" t="s">
         <v>54</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
     </row>
-    <row r="5" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="4"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="12" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="7"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="4"/>
       <c r="N6" s="3"/>
     </row>
-    <row r="7" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="4"/>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="12" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="6"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="4"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="6"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="4"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="4"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="4"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="4"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="M12" s="1"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="9"/>
-      <c r="D13" s="4"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A14" s="4"/>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="8" t="s">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="4"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="4"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="9"/>
-      <c r="D19" s="4"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="8" t="s">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="4"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="8" t="s">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="4"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="4"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="8" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="4"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="M23" s="1"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="8" t="s">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="4"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="8" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="8" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="4"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="4"/>
-      <c r="B27" s="8" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C27" s="9"/>
-      <c r="D27" s="4"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:14" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A28" s="4"/>
-      <c r="B28" s="8" t="s">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="4"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="N28" s="3"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="4"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
       <c r="G29" s="4"/>
@@ -1844,293 +1818,265 @@
       <c r="N29" s="3"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="8" t="s">
+      <c r="A30" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="4"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="N30" s="3"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="4"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
       <c r="G31" s="4"/>
       <c r="N31" s="3"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="12" t="s">
+      <c r="A32" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="4"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="4"/>
       <c r="N32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="8" t="s">
+      <c r="A33" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="4"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="N33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="9"/>
-      <c r="D34" s="4"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="N34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="8" t="s">
+      <c r="A35" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C35" s="9"/>
-      <c r="D35" s="4"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="M35" s="1"/>
       <c r="N35" s="3"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="8" t="s">
+      <c r="A36" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="4"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
       <c r="N36" s="3"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="9"/>
-      <c r="D37" s="4"/>
+      <c r="B37" s="9"/>
+      <c r="C37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="N37" s="3"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
-      <c r="B38" s="8" t="s">
+      <c r="A38" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="4"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="N38" s="3"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="8" t="s">
+      <c r="A39" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="4"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
       <c r="N39" s="3"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="8" t="s">
+      <c r="A40" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="9"/>
-      <c r="D40" s="4"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="N40" s="3"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="8" t="s">
+      <c r="A41" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="9"/>
-      <c r="D41" s="4"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="8" t="s">
+      <c r="A42" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="4"/>
+      <c r="B42" s="9"/>
+      <c r="C42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="8" t="s">
+      <c r="A43" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="9"/>
-      <c r="D43" s="4"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="8" t="s">
+      <c r="A44" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C44" s="9"/>
-      <c r="D44" s="4"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="8" t="s">
+      <c r="A45" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="9"/>
-      <c r="D45" s="4"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="8" t="s">
+      <c r="A46" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C46" s="9"/>
-      <c r="D46" s="4"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="4"/>
-      <c r="B47" s="8" t="s">
+      <c r="A47" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="9"/>
-      <c r="D47" s="4"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="8" t="s">
+      <c r="A48" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="9"/>
-      <c r="D48" s="4"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="4"/>
       <c r="E48" s="4"/>
       <c r="F48" s="4"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="8" t="s">
+      <c r="A49" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="4"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="4"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-      <c r="B51" s="12" t="s">
+      <c r="A51" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="4"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-      <c r="B52" s="5" t="s">
+      <c r="A52" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="9"/>
-      <c r="D52" s="4"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-      <c r="B53" s="5" t="s">
+      <c r="A53" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C53" s="9"/>
-      <c r="D53" s="4"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="5" t="s">
+      <c r="A54" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="9"/>
-      <c r="D54" s="4"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C55" s="9"/>
-      <c r="D55" s="4"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4"/>
-      <c r="B56" s="4" t="s">
+      <c r="A56" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="9"/>
-      <c r="D56" s="4"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="4"/>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
-      <c r="B57" s="5" t="s">
+      <c r="A57" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="4"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="4"/>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
     </row>
@@ -2195,21 +2141,21 @@
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="46"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="54"/>
     </row>
     <row r="4" spans="1:17" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>
@@ -2290,16 +2236,16 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="53" t="s">
+      <c r="C3" s="62"/>
+      <c r="D3" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="53"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="28"/>
@@ -2583,54 +2529,54 @@
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="56" t="s">
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="55"/>
-      <c r="Y3" s="56" t="s">
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="59"/>
+      <c r="Y3" s="60" t="s">
         <v>138</v>
       </c>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="55"/>
-      <c r="AI3" s="54" t="s">
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="59"/>
+      <c r="AI3" s="58" t="s">
         <v>139</v>
       </c>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="54"/>
-      <c r="AM3" s="54"/>
-      <c r="AN3" s="54"/>
-      <c r="AO3" s="54"/>
-      <c r="AP3" s="54"/>
-      <c r="AQ3" s="54"/>
-      <c r="AR3" s="55"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="58"/>
+      <c r="AN3" s="58"/>
+      <c r="AO3" s="58"/>
+      <c r="AP3" s="58"/>
+      <c r="AQ3" s="58"/>
+      <c r="AR3" s="59"/>
       <c r="AS3" s="4"/>
       <c r="AT3" s="4"/>
       <c r="AU3" s="4"/>
@@ -2815,30 +2761,30 @@
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
       <c r="D3" s="44"/>
-      <c r="E3" s="54" t="s">
+      <c r="E3" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="56" t="s">
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="55"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="59"/>
     </row>
     <row r="4" spans="1:24" ht="28.9" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
@@ -2926,7 +2872,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2983,7 +2929,7 @@
   <dimension ref="A1:AA7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3016,114 +2962,114 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="64" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+    <row r="3" spans="1:27" s="52" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="46" t="s">
         <v>83</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="46" t="s">
         <v>147</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="H3" s="59"/>
-      <c r="I3" s="60" t="s">
+      <c r="H3" s="47"/>
+      <c r="I3" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="61" t="s">
+      <c r="J3" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="L3" s="61" t="s">
+      <c r="L3" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="61" t="s">
+      <c r="M3" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="N3" s="61" t="s">
+      <c r="N3" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="61" t="s">
+      <c r="O3" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="P3" s="62" t="s">
+      <c r="P3" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" s="62" t="s">
+      <c r="Q3" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="R3" s="62" t="s">
+      <c r="R3" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="S3" s="62" t="s">
+      <c r="S3" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="T3" s="62" t="s">
+      <c r="T3" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="U3" s="62" t="s">
+      <c r="U3" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="V3" s="62" t="s">
+      <c r="V3" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="W3" s="62" t="s">
+      <c r="W3" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="X3" s="62" t="s">
+      <c r="X3" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="Y3" s="62" t="s">
+      <c r="Y3" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="Z3" s="62" t="s">
+      <c r="Z3" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="AA3" s="63" t="s">
+      <c r="AA3" s="51" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="57"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="45"/>
+      <c r="AA4" s="45"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H5" s="4"/>
@@ -3205,76 +3151,76 @@
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="45" t="s">
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
+      <c r="P3" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="46"/>
-      <c r="AB3" s="47" t="s">
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="54"/>
+      <c r="AB3" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="AC3" s="48"/>
-      <c r="AD3" s="48"/>
-      <c r="AE3" s="48"/>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="49"/>
-      <c r="AN3" s="47" t="s">
+      <c r="AC3" s="56"/>
+      <c r="AD3" s="56"/>
+      <c r="AE3" s="56"/>
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="57"/>
+      <c r="AN3" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="48"/>
-      <c r="AR3" s="48"/>
-      <c r="AS3" s="48"/>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="49"/>
-      <c r="AZ3" s="47" t="s">
+      <c r="AO3" s="56"/>
+      <c r="AP3" s="56"/>
+      <c r="AQ3" s="56"/>
+      <c r="AR3" s="56"/>
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="56"/>
+      <c r="AW3" s="56"/>
+      <c r="AX3" s="56"/>
+      <c r="AY3" s="57"/>
+      <c r="AZ3" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="48"/>
-      <c r="BE3" s="48"/>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="49"/>
+      <c r="BA3" s="56"/>
+      <c r="BB3" s="56"/>
+      <c r="BC3" s="56"/>
+      <c r="BD3" s="56"/>
+      <c r="BE3" s="56"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="57"/>
     </row>
     <row r="4" spans="1:63" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -3508,50 +3454,50 @@
       <c r="A3" s="43"/>
       <c r="B3" s="43"/>
       <c r="C3" s="44"/>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60" t="s">
         <v>128</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="55"/>
-      <c r="V3" s="56" t="s">
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="60" t="s">
         <v>129</v>
       </c>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="55"/>
-      <c r="AE3" s="54" t="s">
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="59"/>
+      <c r="AE3" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="54"/>
-      <c r="AM3" s="55"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="59"/>
       <c r="AN3" s="4"/>
       <c r="AO3" s="4"/>
       <c r="AP3" s="4"/>
@@ -4053,20 +3999,20 @@
       <c r="A3" s="17"/>
       <c r="B3" s="17"/>
       <c r="C3" s="16"/>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="46"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="54"/>
     </row>
     <row r="4" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
@@ -4128,7 +4074,7 @@
   <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+      <selection activeCell="A2" sqref="A2:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,28 +4096,28 @@
       <c r="A3" s="43"/>
       <c r="B3" s="43"/>
       <c r="C3" s="44"/>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="58" t="s">
         <v>133</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="55"/>
-      <c r="M3" s="56" t="s">
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60" t="s">
         <v>134</v>
       </c>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="55"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="59"/>
     </row>
     <row r="4" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
@@ -4300,81 +4246,81 @@
       <c r="B3" s="17"/>
       <c r="C3" s="17"/>
       <c r="D3" s="16"/>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="53" t="s">
         <v>141</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="50" t="s">
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="54"/>
+      <c r="R3" s="61" t="s">
         <v>142</v>
       </c>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="46"/>
-      <c r="AE3" s="47" t="s">
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="54"/>
+      <c r="AE3" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="AF3" s="48"/>
-      <c r="AG3" s="48"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AM3" s="48"/>
-      <c r="AN3" s="48"/>
-      <c r="AO3" s="48"/>
-      <c r="AP3" s="48"/>
-      <c r="AQ3" s="49"/>
-      <c r="AR3" s="47" t="s">
+      <c r="AF3" s="56"/>
+      <c r="AG3" s="56"/>
+      <c r="AH3" s="56"/>
+      <c r="AI3" s="56"/>
+      <c r="AJ3" s="56"/>
+      <c r="AK3" s="56"/>
+      <c r="AL3" s="56"/>
+      <c r="AM3" s="56"/>
+      <c r="AN3" s="56"/>
+      <c r="AO3" s="56"/>
+      <c r="AP3" s="56"/>
+      <c r="AQ3" s="57"/>
+      <c r="AR3" s="55" t="s">
         <v>144</v>
       </c>
-      <c r="AS3" s="48"/>
-      <c r="AT3" s="48"/>
-      <c r="AU3" s="48"/>
-      <c r="AV3" s="48"/>
-      <c r="AW3" s="48"/>
-      <c r="AX3" s="48"/>
-      <c r="AY3" s="48"/>
-      <c r="AZ3" s="48"/>
-      <c r="BA3" s="48"/>
-      <c r="BB3" s="48"/>
-      <c r="BC3" s="48"/>
-      <c r="BD3" s="49"/>
-      <c r="BE3" s="47" t="s">
+      <c r="AS3" s="56"/>
+      <c r="AT3" s="56"/>
+      <c r="AU3" s="56"/>
+      <c r="AV3" s="56"/>
+      <c r="AW3" s="56"/>
+      <c r="AX3" s="56"/>
+      <c r="AY3" s="56"/>
+      <c r="AZ3" s="56"/>
+      <c r="BA3" s="56"/>
+      <c r="BB3" s="56"/>
+      <c r="BC3" s="56"/>
+      <c r="BD3" s="57"/>
+      <c r="BE3" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="BF3" s="48"/>
-      <c r="BG3" s="48"/>
-      <c r="BH3" s="48"/>
-      <c r="BI3" s="48"/>
-      <c r="BJ3" s="48"/>
-      <c r="BK3" s="48"/>
-      <c r="BL3" s="48"/>
-      <c r="BM3" s="48"/>
-      <c r="BN3" s="48"/>
-      <c r="BO3" s="48"/>
-      <c r="BP3" s="48"/>
-      <c r="BQ3" s="49"/>
+      <c r="BF3" s="56"/>
+      <c r="BG3" s="56"/>
+      <c r="BH3" s="56"/>
+      <c r="BI3" s="56"/>
+      <c r="BJ3" s="56"/>
+      <c r="BK3" s="56"/>
+      <c r="BL3" s="56"/>
+      <c r="BM3" s="56"/>
+      <c r="BN3" s="56"/>
+      <c r="BO3" s="56"/>
+      <c r="BP3" s="56"/>
+      <c r="BQ3" s="57"/>
     </row>
     <row r="4" spans="1:69" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A4" s="14"/>

</xml_diff>